<commit_message>
finish artist data, start gathering reception data
</commit_message>
<xml_diff>
--- a/feature_differences.xlsx
+++ b/feature_differences.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ctdin\OneDrive\Documents\Projects\metallica-blacklist-datavis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{F3944FFE-1EE5-4A52-9807-1E4A6E2D0593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D708404E-7CB8-4899-932A-F0204A85DC0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{77341BFF-EBDB-441B-A97E-EBC674A4FDF6}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{77341BFF-EBDB-441B-A97E-EBC674A4FDF6}"/>
   </bookViews>
   <sheets>
     <sheet name="raw_data" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,20 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">raw_data!$A$1:$Y$54</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -829,17 +842,17 @@
     <xf numFmtId="0" fontId="16" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="16" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="16" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="16" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="16" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -16281,7 +16294,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6E5995B-0DA3-432B-874D-22CB49ACC1B7}">
   <dimension ref="A1:Y54"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1:Q1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
@@ -20458,7 +20473,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F97CB77C-7002-4364-A414-23FF37036891}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AI62" sqref="AI62"/>
     </sheetView>
   </sheetViews>

</xml_diff>